<commit_message>
Milira Race Gene Patch 업데이트
#982
</commit_message>
<xml_diff>
--- a/Data/Ancot/Milira Race Gene Patch - 3257000248/3257000248.xlsx
+++ b/Data/Ancot/Milira Race Gene Patch - 3257000248/3257000248.xlsx
@@ -1,26 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.8.6\Milira Race Gene Patch - 3257000248\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Ancot\Milira Race Gene Patch - 3257000248\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C997CA-A866-4D97-B0EA-B0FF2736CEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53745DF-E54B-4030-8DC5-2B80A25CB659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="38340" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240601" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240606" sheetId="3" r:id="rId1"/>
+    <sheet name="Merge_240606" sheetId="2" r:id="rId2"/>
+    <sheet name="Old_240601" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="109">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -284,13 +299,77 @@
   </si>
   <si>
     <t>지식이 풍부한</t>
+  </si>
+  <si>
+    <t>하늘을 날아다니는 고대 종족인 하늘 엘프, 밀리라. 허리에 하얀 날개가 있고 머리 위에는 다양한 모양의 헤일로가 있어 종종 천사로 여겨져 많은 인간에게 숭배를 받아왔습니다.</t>
+  </si>
+  <si>
+    <t>하늘 엘프</t>
+  </si>
+  <si>
+    <t>이 유전자를 가진 사람은 협상 능력이 뛰어납니다.</t>
+  </si>
+  <si>
+    <t>협상가</t>
+  </si>
+  <si>
+    <t>이 유전자를 가진 사람은 기계를 만지는 데 뛰어난 능력을 가지고 있습니다.</t>
+  </si>
+  <si>
+    <t>기계 지식</t>
+  </si>
+  <si>
+    <t>이 유전자를 가진 사람은 일을 끝내는 것보다 우아하게 보이는 것에 더 신경을 씁니다.</t>
+  </si>
+  <si>
+    <t>여유로움</t>
+  </si>
+  <si>
+    <t>지식</t>
+  </si>
+  <si>
+    <t>똑똑함</t>
+  </si>
+  <si>
+    <t>기억</t>
+  </si>
+  <si>
+    <t>연구자</t>
+  </si>
+  <si>
+    <t>지혜</t>
+  </si>
+  <si>
+    <t>박사</t>
+  </si>
+  <si>
+    <t>괴짜</t>
+  </si>
+  <si>
+    <t>두뇌</t>
+  </si>
+  <si>
+    <t>이 유전자를 가진 사람은 학습 및 연구 속도가 빠릅니다.</t>
+  </si>
+  <si>
+    <t>지식욕</t>
+  </si>
+  <si>
+    <t>이 유전자를 가진 사람은 더러운 환경을 싫어하고 청소하는 데 더 많은 시간을 소비합니다.</t>
+  </si>
+  <si>
+    <t>결벽증</t>
+  </si>
+  <si>
+    <t>Index_240606</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -309,16 +388,30 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -326,15 +419,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="셀 확인" xfId="1" builtinId="23"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -634,10 +747,783 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BA4CD2-85B2-4CCA-81A0-281DB8A93B52}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="66.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737E3ADE-E7D6-4FF5-87E9-083191097EB0}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="66.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>IF(B2="",A2,B2)</f>
+        <v>GeneCategoryDef+Milira_GeneCategory.label</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="1">
+        <f>MATCH(C2,Main_240606!$A$2:$A$22,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C22" si="0">IF(B3="",A3,B3)</f>
+        <v>GeneDef+Milira_Ablutomania.label</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="1">
+        <f>MATCH(C3,Main_240606!$A$2:$A$22,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Ablutomania.description</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="1">
+        <f>MATCH(C4,Main_240606!$A$2:$A$22,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.label</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="1">
+        <f>MATCH(C5,Main_240606!$A$2:$A$22,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.description</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="1">
+        <f>MATCH(C6,Main_240606!$A$2:$A$22,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.symbolPack.prefixSymbols.0.symbol</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="1">
+        <f>MATCH(C7,Main_240606!$A$2:$A$22,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.symbolPack.prefixSymbols.1.symbol</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="1">
+        <f>MATCH(C8,Main_240606!$A$2:$A$22,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.symbolPack.prefixSymbols.2.symbol</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="1">
+        <f>MATCH(C9,Main_240606!$A$2:$A$22,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.symbolPack.prefixSymbols.3.symbol</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1">
+        <f>MATCH(C10,Main_240606!$A$2:$A$22,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.symbolPack.prefixSymbols.4.symbol</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="1">
+        <f>MATCH(C11,Main_240606!$A$2:$A$22,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.symbolPack.prefixSymbols.5.symbol</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="1">
+        <f>MATCH(C12,Main_240606!$A$2:$A$22,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.symbolPack.suffixSymbols.0.symbol</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="1">
+        <f>MATCH(C13,Main_240606!$A$2:$A$22,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Knowledgeable.symbolPack.suffixSymbols.1.symbol</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="1">
+        <f>MATCH(C14,Main_240606!$A$2:$A$22,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Leisurely.label</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="1">
+        <f>MATCH(C15,Main_240606!$A$2:$A$22,0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Leisurely.description</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="1">
+        <f>MATCH(C16,Main_240606!$A$2:$A$22,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Mechining.label</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="1">
+        <f>MATCH(C17,Main_240606!$A$2:$A$22,0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_Mechining.description</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="1">
+        <f>MATCH(C18,Main_240606!$A$2:$A$22,0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_ProNegotiator.label</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="1">
+        <f>MATCH(C19,Main_240606!$A$2:$A$22,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GeneDef+Milira_ProNegotiator.description</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="1">
+        <f>MATCH(C20,Main_240606!$A$2:$A$22,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>XenotypeDef+MiliraXenotype.label</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="1">
+        <f>MATCH(C21,Main_240606!$A$2:$A$22,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>XenotypeDef+MiliraXenotype.description</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="1">
+        <f>MATCH(C22,Main_240606!$A$2:$A$22,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>